<commit_message>
atualizacao de bugun agora agindo de forma esperada
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aalui\python\editandopdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto-certificados-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE68DD36-9EC4-4C34-BA30-65B5864E5C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE24CE1-00B6-4438-96BC-7E3C52445093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{09868F48-6BDF-4DB9-A918-4AF881DA5910}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{09868F48-6BDF-4DB9-A918-4AF881DA5910}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Alunos</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>marido da mulher que vende cheiro verde</t>
+  </si>
+  <si>
+    <t>ana maria dos santos</t>
+  </si>
+  <si>
+    <t>isa gabrielly de oliveira</t>
+  </si>
+  <si>
+    <t>seu maico de aumenda</t>
   </si>
 </sst>
 </file>
@@ -215,9 +224,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -255,7 +264,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -361,7 +370,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -503,7 +512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -511,21 +520,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85B4A0E-F78A-4C63-82F6-9752EFC34C12}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
-    <col min="4" max="6" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -559,7 +568,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -576,7 +585,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -593,7 +602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -610,7 +619,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -627,7 +636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -644,7 +653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -661,7 +670,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -678,7 +687,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -695,7 +704,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -712,7 +721,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -729,7 +738,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -744,6 +753,57 @@
       </c>
       <c r="E13">
         <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>